<commit_message>
Jigsaw : limit modules
</commit_message>
<xml_diff>
--- a/java/java9/jigsaw/doc/images.xlsx
+++ b/java/java9/jigsaw/doc/images.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="java.seに内モジュール" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">java.seに内モジュール!$A$1:$C$28</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="114">
   <si>
     <t>java.se</t>
     <phoneticPr fontId="1"/>
@@ -420,6 +424,130 @@
     <rPh sb="7" eb="9">
       <t>キドウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">java.se </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>以外の全</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> java.* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>モジュール</t>
+    </r>
+    <rPh sb="8" eb="10">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ゼン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">java.se </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>が</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> transitive </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>しているモジュール</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>非推奨</t>
+    <rPh sb="0" eb="3">
+      <t>ヒスイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Java Web Start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>関係のパッケージ</t>
+    </r>
+    <rPh sb="14" eb="16">
+      <t>カンケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>スマート・カード入出力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>API</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -544,11 +672,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -904,10 +1032,10 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" s="5"/>
@@ -944,622 +1072,622 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B99" sqref="B99:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="39.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+      <c r="A87" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+      <c r="A91" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+      <c r="A95" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="9" t="s">
+      <c r="A99" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="8" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1568,4 +1696,254 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C28">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>